<commit_message>
Zuhayr: Added more frequency response measurements for the bode plot.
</commit_message>
<xml_diff>
--- a/Prac2/eee3096_prac2.xlsx
+++ b/Prac2/eee3096_prac2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uctcloud-my.sharepoint.com/personal/hldzuh001_myuct_ac_za/Documents/UCT/3rd Year/2nd Semester/EEE3096S/Practicals/Practical 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uctcloud-my.sharepoint.com/personal/hldzuh001_myuct_ac_za/Documents/UCT/3rd Year/2nd Semester/EEE3096S/Practicals/HLDZUH001_KSHKAV001_EEE3096S/Prac2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{FD59CEC1-F89D-4521-91FA-3EC655D990D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C145F27-F590-4548-903B-30CE61072433}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{FD59CEC1-F89D-4521-91FA-3EC655D990D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C863511F-BC90-44E1-9F0C-78FAE2F2CEF3}"/>
   <bookViews>
     <workbookView xWindow="2138" yWindow="248" windowWidth="16200" windowHeight="9847" xr2:uid="{F1AEC267-DAE4-4A4C-A435-25FC174C88B1}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Attentuation</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Frequency</t>
   </si>
@@ -97,6 +94,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -416,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7B3C76-5BFA-4C29-BDC9-9949727B30B1}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -429,231 +430,180 @@
     <col min="3" max="3" width="13.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>3.24</v>
       </c>
       <c r="B2">
         <v>50</v>
       </c>
-      <c r="C2">
-        <f>ROUND(A2/5,2)</f>
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>3.16</v>
       </c>
       <c r="B3">
         <v>150</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C19" si="0">ROUND(A3/5,2)</f>
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3.08</v>
       </c>
       <c r="B4">
         <v>250</v>
       </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>0.62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>2.97</v>
       </c>
       <c r="B5">
         <v>350</v>
       </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2.89</v>
       </c>
       <c r="B6">
         <v>450</v>
       </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>0.57999999999999996</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>2.77</v>
       </c>
       <c r="B7">
         <v>550</v>
       </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>2.63</v>
       </c>
       <c r="B8">
         <v>650</v>
       </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>0.53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>2.5499999999999998</v>
       </c>
       <c r="B9">
         <v>750</v>
       </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>2.4300000000000002</v>
       </c>
       <c r="B10">
         <v>850</v>
       </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>0.49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>2.33</v>
       </c>
       <c r="B11">
         <v>950</v>
       </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>2.25</v>
       </c>
       <c r="B12">
         <v>1050</v>
       </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>2.17</v>
       </c>
       <c r="B13">
         <v>1150</v>
       </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>2.0699999999999998</v>
       </c>
       <c r="B14">
         <v>1250</v>
       </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>0.41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>1.99</v>
       </c>
       <c r="B15">
         <v>1350</v>
       </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>1.93</v>
       </c>
       <c r="B16">
         <v>1450</v>
       </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>1.79</v>
       </c>
       <c r="B17">
         <v>1550</v>
       </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>1.79</v>
       </c>
       <c r="B18">
         <v>1650</v>
       </c>
-      <c r="C18">
-        <f t="shared" si="0"/>
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>1.75</v>
       </c>
       <c r="B19">
         <v>1750</v>
       </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
-        <v>0.35</v>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>1.7</v>
+      </c>
+      <c r="B20">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>1.5</v>
+      </c>
+      <c r="B21">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B22">
+        <v>4000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>